<commit_message>
update sms gateway dan akademik03122023LenovoLihit.sql
</commit_message>
<xml_diff>
--- a/template-phonebook.xlsx
+++ b/template-phonebook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp5640\htdocs\learn_akademik\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp_ver5\htdocs\learn_akademik\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{976DB69A-80D3-4E4E-B15C-31FFE8261936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E49FC20-5E4F-4DB5-A141-295E356A99CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{33B9EB31-46D3-41DA-8816-FCA5F7E7D5AB}"/>
+    <workbookView xWindow="6810" yWindow="6615" windowWidth="12600" windowHeight="7155" xr2:uid="{33B9EB31-46D3-41DA-8816-FCA5F7E7D5AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,54 +36,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Nomor Handphone</t>
-  </si>
-  <si>
-    <t>Keterangan</t>
-  </si>
-  <si>
-    <t>Nama</t>
-  </si>
-  <si>
-    <t>Daftar Nomor Handphone</t>
-  </si>
-  <si>
-    <t>Muhammad Huzaifah</t>
-  </si>
-  <si>
-    <t>Rachmah Octarina</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>081386745521</t>
   </si>
   <si>
-    <t>081311803778</t>
+    <t>No_HP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -95,7 +66,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -103,34 +74,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,94 +396,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73741C5E-B85B-4F75-8E60-290FF5D6CB32}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>